<commit_message>
update API save file
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -460,7 +460,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bảng cần đổi kế toán riêng</t>
+          <t>Bảng cân đối kế toán riêng</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -489,7 +489,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>11.12</t>
+          <t>11-12</t>
         </is>
       </c>
     </row>
@@ -508,12 +508,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Phụ lực 1 - Danh sách cống ty con tại ngày 31 tháng 12 năm 2022</t>
+          <t>Phụ lục 1 - Danh sách công ty con tại ngày 31 tháng 12 năm 2022</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>80 - 83</t>
+          <t>80.83</t>
         </is>
       </c>
     </row>

</xml_diff>